<commit_message>
Otimizando e colocando dcumentações
</commit_message>
<xml_diff>
--- a/Planilha/Planilha.xlsx
+++ b/Planilha/Planilha.xlsx
@@ -3724,7 +3724,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5198,7 +5198,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5339,11 +5339,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="73080809"/>
-        <c:axId val="36226206"/>
+        <c:axId val="70428782"/>
+        <c:axId val="74150235"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73080809"/>
+        <c:axId val="70428782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5412,7 +5412,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36226206"/>
+        <c:crossAx val="74150235"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5420,7 +5420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36226206"/>
+        <c:axId val="74150235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5499,7 +5499,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73080809"/>
+        <c:crossAx val="70428782"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5552,7 +5552,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5688,11 +5688,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="64924088"/>
-        <c:axId val="31094654"/>
+        <c:axId val="53025679"/>
+        <c:axId val="48165686"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64924088"/>
+        <c:axId val="53025679"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5761,7 +5761,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31094654"/>
+        <c:crossAx val="48165686"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5769,7 +5769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31094654"/>
+        <c:axId val="48165686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5812,7 +5812,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64924088"/>
+        <c:crossAx val="53025679"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5865,7 +5865,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6001,11 +6001,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="71472924"/>
-        <c:axId val="38314784"/>
+        <c:axId val="90868936"/>
+        <c:axId val="69088053"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71472924"/>
+        <c:axId val="90868936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6074,7 +6074,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38314784"/>
+        <c:crossAx val="69088053"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6082,7 +6082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38314784"/>
+        <c:axId val="69088053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6125,7 +6125,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71472924"/>
+        <c:crossAx val="90868936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>